<commit_message>
feat(app): add items on commande
</commit_message>
<xml_diff>
--- a/LBS-stories-2021-22.xlsx
+++ b/LBS-stories-2021-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIASIE\NodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B767A7-32F4-422D-BA74-09FB3A8AFF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6998BFFE-A25D-453A-A49E-643586716BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>http://localhost:3000/commandes/:id</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/commandes/:id/items</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -864,8 +867,12 @@
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>71</v>
+      </c>
       <c r="F7" s="16" t="s">
         <v>14</v>
       </c>
@@ -29006,6 +29013,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{98167DBA-15C0-4F26-9020-912A63F0FE00}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{B5B10F2F-B1DC-40E4-BF0A-4C9A199A83D5}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
feat(other): add stuff on excel
</commit_message>
<xml_diff>
--- a/LBS-stories-2021-22.xlsx
+++ b/LBS-stories-2021-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIASIE\NodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6998BFFE-A25D-453A-A49E-643586716BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD98219-EBE5-4D85-AD5E-FB5DB7E6B33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -252,6 +252,15 @@
   <si>
     <t>http://localhost:3000/commandes/:id/items</t>
   </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/commandes</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/commandes/:id?token=XXX</t>
+  </si>
 </sst>
 </file>
 
@@ -348,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,9 +392,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -639,7 +645,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -826,36 +832,36 @@
       <c r="D6" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="13">
         <v>3</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="32.25" customHeight="1">
       <c r="A7" s="12">
@@ -870,36 +876,36 @@
       <c r="D7" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="13">
         <v>3</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="32.25" customHeight="1">
       <c r="A8" s="12" t="s">
@@ -911,35 +917,39 @@
       <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16" t="s">
+      <c r="D8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="13">
         <v>4</v>
       </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="32.25" customHeight="1">
       <c r="A9" s="12">
@@ -951,35 +961,39 @@
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="13">
         <v>4</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="32.25" customHeight="1">
       <c r="A10" s="12" t="s">
@@ -991,35 +1005,39 @@
       <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="20" t="s">
+      <c r="D10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="13">
         <v>2</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="17"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="17"/>
-      <c r="Z10" s="17"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="32.25" customHeight="1">
       <c r="A11" s="12" t="s">
@@ -1031,53 +1049,57 @@
       <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20" t="s">
+      <c r="D11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="13">
         <v>4</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
     </row>
     <row r="12" spans="1:26" ht="47.25" customHeight="1">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>104</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="13">
         <v>2</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <v>4</v>
       </c>
       <c r="I12" s="3"/>
@@ -1100,14 +1122,14 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1200,24 +1222,24 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="47.25" customHeight="1">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>201</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20" t="s">
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="20">
         <v>3</v>
       </c>
       <c r="I16" s="3"/>
@@ -1240,24 +1262,24 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="24" customHeight="1">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>202</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="20">
         <v>4</v>
       </c>
       <c r="I17" s="3"/>
@@ -1280,22 +1302,22 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A18" s="21">
+      <c r="A18" s="20">
         <v>203</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="20">
         <v>2</v>
       </c>
       <c r="I18" s="3"/>
@@ -1318,22 +1340,22 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="24" customHeight="1">
-      <c r="A19" s="21">
+      <c r="A19" s="20">
         <v>204</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="13">
         <v>2</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="20">
         <v>4</v>
       </c>
       <c r="I19" s="3"/>
@@ -1356,14 +1378,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="24.75" customHeight="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="21"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1456,18 +1478,18 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A23" s="23">
+      <c r="A23" s="22">
         <v>301</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="24" t="s">
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -1496,24 +1518,24 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="30.75" customHeight="1">
-      <c r="A24" s="21">
+      <c r="A24" s="20">
         <v>302</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="13">
         <v>1</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20" t="s">
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H24" s="20">
         <v>6</v>
       </c>
       <c r="I24" s="3"/>
@@ -1536,22 +1558,22 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="24.75" customHeight="1">
-      <c r="A25" s="21">
+      <c r="A25" s="20">
         <v>303</v>
       </c>
-      <c r="B25" s="21"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="13">
         <v>3</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20" t="s">
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="20">
         <v>6</v>
       </c>
       <c r="I25" s="3"/>
@@ -1581,8 +1603,8 @@
       <c r="C26" s="2">
         <v>2</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1712,24 +1734,24 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <v>401</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="13">
         <v>1</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="24" t="s">
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="23" t="s">
         <v>42</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="21">
+      <c r="H30" s="20">
         <v>4</v>
       </c>
       <c r="I30" s="3"/>
@@ -1752,24 +1774,24 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="47.25" customHeight="1">
-      <c r="A31" s="21">
+      <c r="A31" s="20">
         <v>402</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="13">
         <v>1</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20" t="s">
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="21">
+      <c r="H31" s="20">
         <v>6</v>
       </c>
       <c r="I31" s="3"/>
@@ -1892,24 +1914,24 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A35" s="21">
+      <c r="A35" s="20">
         <v>501</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="13">
         <v>1</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20" t="s">
+      <c r="D35" s="17"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="21">
+      <c r="H35" s="20">
         <v>5</v>
       </c>
       <c r="I35" s="3"/>
@@ -1932,24 +1954,24 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A36" s="21">
+      <c r="A36" s="20">
         <v>502</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="13">
         <v>1</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20" t="s">
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="20">
         <v>5</v>
       </c>
       <c r="I36" s="3"/>
@@ -1972,22 +1994,22 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A37" s="21">
+      <c r="A37" s="20">
         <v>503</v>
       </c>
-      <c r="B37" s="21"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="13">
         <v>2</v>
       </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20" t="s">
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H37" s="21">
+      <c r="H37" s="20">
         <v>4</v>
       </c>
       <c r="I37" s="3"/>
@@ -2010,24 +2032,24 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="35.25" customHeight="1">
-      <c r="A38" s="21">
+      <c r="A38" s="20">
         <v>504</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>62</v>
       </c>
       <c r="C38" s="13">
         <v>1</v>
       </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20" t="s">
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="21">
+      <c r="H38" s="20">
         <v>8</v>
       </c>
       <c r="I38" s="3"/>
@@ -2050,22 +2072,22 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A39" s="21">
+      <c r="A39" s="20">
         <v>505</v>
       </c>
-      <c r="B39" s="21"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="13">
         <v>3</v>
       </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20" t="s">
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H39" s="21">
+      <c r="H39" s="20">
         <v>3</v>
       </c>
       <c r="I39" s="3"/>
@@ -2088,22 +2110,22 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A40" s="21">
+      <c r="A40" s="20">
         <v>506</v>
       </c>
-      <c r="B40" s="21"/>
+      <c r="B40" s="20"/>
       <c r="C40" s="13">
         <v>3</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20" t="s">
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="21">
+      <c r="H40" s="20">
         <v>3</v>
       </c>
       <c r="I40" s="3"/>
@@ -2126,14 +2148,14 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="24" customHeight="1">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
       <c r="C41" s="13"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="21"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="20"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2215,8 +2237,8 @@
       <c r="C44" s="2"/>
       <c r="D44" s="1"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
       <c r="H44" s="1"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -2243,8 +2265,8 @@
       <c r="C45" s="2"/>
       <c r="D45" s="1"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
       <c r="H45" s="1"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -2271,8 +2293,8 @@
       <c r="C46" s="2"/>
       <c r="D46" s="1"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
       <c r="H46" s="1"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -2299,8 +2321,8 @@
       <c r="C47" s="2"/>
       <c r="D47" s="1"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="27" t="s">
+      <c r="F47" s="23"/>
+      <c r="G47" s="26" t="s">
         <v>68</v>
       </c>
       <c r="H47" s="1">
@@ -29014,6 +29036,10 @@
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{98167DBA-15C0-4F26-9020-912A63F0FE00}"/>
     <hyperlink ref="E7" r:id="rId2" xr:uid="{B5B10F2F-B1DC-40E4-BF0A-4C9A199A83D5}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{78952B69-FB0C-421F-A19B-4AD3BDA4719C}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{F2BF8638-1C7B-4E27-AB70-B6AF5BBB9B46}"/>
+    <hyperlink ref="E11" r:id="rId5" xr:uid="{79C8290A-6BC9-463C-869B-C45AAFCAA4D9}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{B0F7ED0B-48F0-4E6B-92B1-870ADF5D994F}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
feat(app): update excel & add order by on /commandes
</commit_message>
<xml_diff>
--- a/LBS-stories-2021-22.xlsx
+++ b/LBS-stories-2021-22.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIASIE\NodeJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604843AB-8EEE-4B4B-8C0C-97B29F1782A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD35234-6EB2-463D-B3DF-B6EE5C6E816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>http://localhost:3000/commandes/:id?token=XXX</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/commandes?page=1&amp;size=10</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/commandes?s=3</t>
   </si>
 </sst>
 </file>
@@ -644,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1232,7 +1238,9 @@
         <v>1</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="27" t="s">
+        <v>76</v>
+      </c>
       <c r="F16" s="19" t="s">
         <v>32</v>
       </c>
@@ -1272,7 +1280,9 @@
         <v>1</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="27" t="s">
+        <v>75</v>
+      </c>
       <c r="F17" s="19" t="s">
         <v>34</v>
       </c>
@@ -29040,8 +29050,10 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{F2BF8638-1C7B-4E27-AB70-B6AF5BBB9B46}"/>
     <hyperlink ref="E11" r:id="rId5" xr:uid="{79C8290A-6BC9-463C-869B-C45AAFCAA4D9}"/>
     <hyperlink ref="E10" r:id="rId6" xr:uid="{B0F7ED0B-48F0-4E6B-92B1-870ADF5D994F}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{747667D0-63EA-4ADE-BFD8-2CEB4A80FCB4}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{2689E2FC-5759-4186-A607-57DB21B908D9}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update excel & install packages
</commit_message>
<xml_diff>
--- a/LBS-stories-2021-22.xlsx
+++ b/LBS-stories-2021-22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CIASIE\NodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucassaker/Documents/Cours/NodeJS/DevBackEndNodeJS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD35234-6EB2-463D-B3DF-B6EE5C6E816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725AC19F-05A8-2945-B163-9B2E7354CB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -267,6 +267,21 @@
   <si>
     <t>http://localhost:3001/commandes?s=3</t>
   </si>
+  <si>
+    <t>http://localhost:3001/auth/signup</t>
+  </si>
+  <si>
+    <t>http://localhost:3001/auth/signin</t>
+  </si>
+  <si>
+    <t>http://localhost:3002/signin</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:8055/items/sandwich</t>
+  </si>
+  <si>
+    <t>http://0.0.0.0:8055/items/Category</t>
+  </si>
 </sst>
 </file>
 
@@ -363,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -425,13 +440,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -650,19 +666,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="118.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="118.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1">
@@ -838,7 +854,7 @@
       <c r="D6" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="26" t="s">
         <v>70</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -882,7 +898,7 @@
       <c r="D7" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="15" t="s">
@@ -926,7 +942,7 @@
       <c r="D8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>70</v>
       </c>
       <c r="F8" s="15" t="s">
@@ -970,7 +986,7 @@
       <c r="D9" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>73</v>
       </c>
       <c r="F9" s="19" t="s">
@@ -1014,7 +1030,7 @@
       <c r="D10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="26" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="19" t="s">
@@ -1058,7 +1074,7 @@
       <c r="D11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="26" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="19" t="s">
@@ -1238,7 +1254,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="26" t="s">
         <v>76</v>
       </c>
       <c r="F16" s="19" t="s">
@@ -1280,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="26" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="19" t="s">
@@ -1498,7 +1514,9 @@
         <v>1</v>
       </c>
       <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
+      <c r="E23" s="28" t="s">
+        <v>78</v>
+      </c>
       <c r="F23" s="23" t="s">
         <v>42</v>
       </c>
@@ -1614,7 +1632,9 @@
         <v>2</v>
       </c>
       <c r="D26" s="24"/>
-      <c r="E26" s="25"/>
+      <c r="E26" s="27" t="s">
+        <v>77</v>
+      </c>
       <c r="F26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1754,7 +1774,9 @@
         <v>1</v>
       </c>
       <c r="D30" s="17"/>
-      <c r="E30" s="18"/>
+      <c r="E30" s="28" t="s">
+        <v>79</v>
+      </c>
       <c r="F30" s="23" t="s">
         <v>42</v>
       </c>
@@ -1974,7 +1996,9 @@
         <v>1</v>
       </c>
       <c r="D36" s="17"/>
-      <c r="E36" s="18"/>
+      <c r="E36" s="28" t="s">
+        <v>80</v>
+      </c>
       <c r="F36" s="19" t="s">
         <v>58</v>
       </c>
@@ -2012,7 +2036,9 @@
         <v>2</v>
       </c>
       <c r="D37" s="17"/>
-      <c r="E37" s="18"/>
+      <c r="E37" s="28" t="s">
+        <v>81</v>
+      </c>
       <c r="F37" s="19" t="s">
         <v>60</v>
       </c>
@@ -2332,7 +2358,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="3"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="26" t="s">
+      <c r="G47" s="25" t="s">
         <v>68</v>
       </c>
       <c r="H47" s="1">
@@ -29052,8 +29078,13 @@
     <hyperlink ref="E10" r:id="rId6" xr:uid="{B0F7ED0B-48F0-4E6B-92B1-870ADF5D994F}"/>
     <hyperlink ref="E17" r:id="rId7" xr:uid="{747667D0-63EA-4ADE-BFD8-2CEB4A80FCB4}"/>
     <hyperlink ref="E16" r:id="rId8" xr:uid="{2689E2FC-5759-4186-A607-57DB21B908D9}"/>
+    <hyperlink ref="E26" r:id="rId9" xr:uid="{4CE4B844-71AC-EC49-B59E-93666FB2F1EE}"/>
+    <hyperlink ref="E23" r:id="rId10" xr:uid="{28CE3D62-6BDF-F644-B59A-4A9730A2B029}"/>
+    <hyperlink ref="E30" r:id="rId11" xr:uid="{E5C8EFA5-7BC2-8B45-97F3-4CC9917C5B38}"/>
+    <hyperlink ref="E36" r:id="rId12" xr:uid="{FE3F1B99-7D53-E242-9159-C3F6EFA0F895}"/>
+    <hyperlink ref="E37" r:id="rId13" xr:uid="{79D104FD-EC26-2A41-B38A-BBC1F7A4C4FB}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>